<commit_message>
Add results intraday complete
</commit_message>
<xml_diff>
--- a/Comparison_models_intraday.xlsx
+++ b/Comparison_models_intraday.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\33637\Documents\11. Deep Learning\2. Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4FA938A8-BDAA-4002-97CD-296A8B36947F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD4484DC-5D9B-4B44-9CF2-FDD99D7B03BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{C9DEC9D8-A29E-4EA7-8AC0-6E0D2423C727}"/>
   </bookViews>
@@ -34,14 +34,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="24">
   <si>
     <t>AR(3)</t>
   </si>
   <si>
-    <t>FFNN</t>
-  </si>
-  <si>
     <t>LSTM AR(24)</t>
   </si>
   <si>
@@ -49,6 +46,66 @@
   </si>
   <si>
     <t>Persistent</t>
+  </si>
+  <si>
+    <t>RMSE 1h</t>
+  </si>
+  <si>
+    <t>RMSE 2h</t>
+  </si>
+  <si>
+    <t>RMSE 3h</t>
+  </si>
+  <si>
+    <t>RMSE 4h</t>
+  </si>
+  <si>
+    <t>RMSE 5h</t>
+  </si>
+  <si>
+    <t>RMSE 6h</t>
+  </si>
+  <si>
+    <t>FFNN (all hours)</t>
+  </si>
+  <si>
+    <t>FFNN (1h)</t>
+  </si>
+  <si>
+    <t>FFNN (2h)</t>
+  </si>
+  <si>
+    <t>FFNN (3h)</t>
+  </si>
+  <si>
+    <t>FFNN (4h)</t>
+  </si>
+  <si>
+    <t>FFNN (5h)</t>
+  </si>
+  <si>
+    <t>FFNN (6h)</t>
+  </si>
+  <si>
+    <t>MAE 1h</t>
+  </si>
+  <si>
+    <t>MAE 2h</t>
+  </si>
+  <si>
+    <t>MAE 3h</t>
+  </si>
+  <si>
+    <t>MAE 4h</t>
+  </si>
+  <si>
+    <t>MAE 5h</t>
+  </si>
+  <si>
+    <t>MAE 6h</t>
+  </si>
+  <si>
+    <t>NA</t>
   </si>
 </sst>
 </file>
@@ -58,10 +115,24 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -108,11 +179,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -427,10 +502,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EA19094-64B6-4B8E-A5F0-541E6F7E401E}">
-  <dimension ref="A1:G5"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -438,119 +513,494 @@
     <col min="1" max="1" width="45.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A1" s="3"/>
+      <c r="B1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="2">
+      <c r="C1" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M1" s="6" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1">
         <v>7.1999999999999995E-2</v>
       </c>
-      <c r="C1" s="2">
+      <c r="C2" s="1">
         <v>0.114</v>
       </c>
-      <c r="D1" s="2">
-        <v>1.43E-2</v>
-      </c>
-      <c r="E1" s="2">
+      <c r="D2" s="1">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="E2" s="1">
         <v>0.16700000000000001</v>
       </c>
-      <c r="F1" s="2">
+      <c r="F2" s="1">
         <v>0.188</v>
       </c>
-      <c r="G1" s="2">
+      <c r="G2" s="1">
         <v>0.20499999999999999</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="H2" s="3">
+        <v>4.7E-2</v>
+      </c>
+      <c r="I2" s="3">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="J2" s="3">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="K2" s="3">
+        <v>0.114</v>
+      </c>
+      <c r="L2" s="3">
+        <v>0.129</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0.14299999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A3" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B3" s="3">
         <v>6.9000000000000006E-2</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C3" s="4">
         <v>0.11</v>
       </c>
-      <c r="D2">
+      <c r="D3" s="3">
         <v>0.13700000000000001</v>
       </c>
-      <c r="E2">
+      <c r="E3" s="3">
         <v>0.158</v>
       </c>
-      <c r="F2">
+      <c r="F3" s="3">
         <v>0.17599999999999999</v>
       </c>
-      <c r="G2">
+      <c r="G3" s="3">
         <v>0.221</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="H3" s="3">
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="I3" s="3">
+        <v>7.9000000000000001E-2</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="K3" s="3">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="L3" s="3">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="M3" s="3">
+        <v>0.14699999999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="4">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="C4" s="3">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="D4" s="3">
+        <v>0.153</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="F4" s="3">
+        <v>0.20399999999999999</v>
+      </c>
+      <c r="G4" s="7">
+        <v>0.221</v>
+      </c>
+      <c r="H4" s="3">
+        <v>4.7E-2</v>
+      </c>
+      <c r="I4" s="3">
+        <v>7.8E-2</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.10100000000000001</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.11899999999999999</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="M4" s="3">
+        <v>0.14599999999999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1">
-        <v>7.2999999999999995E-2</v>
-      </c>
-      <c r="C3">
-        <v>0.11899999999999999</v>
-      </c>
-      <c r="D3">
-        <v>0.153</v>
-      </c>
-      <c r="E3">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="F3">
-        <v>0.20399999999999999</v>
-      </c>
-      <c r="G3">
+      <c r="B5" s="1">
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="C5" s="1">
+        <v>9.9000000000000005E-2</v>
+      </c>
+      <c r="D5" s="1">
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="E5" s="2">
+        <v>0.13</v>
+      </c>
+      <c r="F5" s="1">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="G5" s="1">
         <v>0.14399999999999999</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2">
-        <v>6.6000000000000003E-2</v>
-      </c>
-      <c r="C4" s="2">
-        <v>9.9000000000000005E-2</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0.11799999999999999</v>
-      </c>
-      <c r="E4" s="3">
-        <v>0.13</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.13900000000000001</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.14399999999999999</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="2">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0.16800000000000001</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0.16800000000000001</v>
+      <c r="H5" s="3">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="I5" s="4">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="J5" s="3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="K5" s="3">
+        <v>9.6000000000000002E-2</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0.10299999999999999</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0.107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A6" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B6" s="1">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="D6" s="1">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="E6" s="1">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="F6" s="1">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0.122</v>
+      </c>
+      <c r="I6" s="3">
+        <v>0.122</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.122</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0.122</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0.122</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0.122</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A7" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="3">
+        <v>0.158</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="3">
+        <v>0.122</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M7" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A8" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C8" s="3">
+        <v>0.161</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I8" s="3">
+        <v>0.124</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L8" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M8" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A9" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" s="3">
+        <v>0.161</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.124</v>
+      </c>
+      <c r="K9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A10" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M10" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A11" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F11" s="3">
+        <v>0.16200000000000001</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0.125</v>
+      </c>
+      <c r="M11" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A12" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" s="3">
+        <v>0.159</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="K12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="L12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0.123</v>
       </c>
     </row>
   </sheetData>

</xml_diff>